<commit_message>
Prepare to merge into main
</commit_message>
<xml_diff>
--- a/ACS_Exam_Scores.xlsx
+++ b/ACS_Exam_Scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewrowley1\Documents\Teaching_Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781EAA1C-C550-4620-9A83-61DE9A6857D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E12807-1FB1-4080-B98D-080C59CA81A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24825" activeTab="3" xr2:uid="{013C798E-9924-44FB-85F0-D0CA2EC3A4F8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24825" activeTab="1" xr2:uid="{013C798E-9924-44FB-85F0-D0CA2EC3A4F8}"/>
   </bookViews>
   <sheets>
     <sheet name="1110" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Lookup table</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>score</t>
+  </si>
+  <si>
+    <t>Lookup Table</t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
   <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,14 +913,431 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A64C594-CC0D-4550-9573-86D004C2C976}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>41</v>
+      </c>
+      <c r="B12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -940,7 +1360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94EA68A9-4AE3-42B9-B0C2-FD343F0E832E}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>